<commit_message>
Data Updated for PDP Preferred
Data Updated for PDP Preferred
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_PDP_Preferred_2022.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_PDP_Preferred_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358F0DB3-4D9A-4F93-89A8-971A40C606A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31D52BE-9CF4-4288-BFB3-7E5B8191010B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" firstSheet="7" activeTab="10" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
   <sheets>
     <sheet name="PDP_Preferred" sheetId="4" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="509">
   <si>
     <t>Link Parameters</t>
   </si>
@@ -1973,9 +1973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D150B402-BA8E-4A98-8F02-52FA07D02190}">
   <dimension ref="A1:AF104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61:AF70"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101:AF104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -12196,13 +12196,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A8DD14-E1DA-4830-9A92-F21A9F938BFD}">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -12300,6 +12300,1476 @@
       </c>
       <c r="AF1" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H2" s="7">
+        <v>25.2</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>15</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>45</v>
+      </c>
+      <c r="M2" s="6">
+        <v>10</v>
+      </c>
+      <c r="N2" s="6">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6">
+        <v>30</v>
+      </c>
+      <c r="P2" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>40</v>
+      </c>
+      <c r="R2" s="6">
+        <v>45</v>
+      </c>
+      <c r="S2" s="6">
+        <v>120</v>
+      </c>
+      <c r="T2" s="6">
+        <v>135</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA2" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC2" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H3" s="7">
+        <v>27.6</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>15</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>45</v>
+      </c>
+      <c r="M3" s="6">
+        <v>10</v>
+      </c>
+      <c r="N3" s="6">
+        <v>20</v>
+      </c>
+      <c r="O3" s="6">
+        <v>30</v>
+      </c>
+      <c r="P3" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>40</v>
+      </c>
+      <c r="R3" s="6">
+        <v>45</v>
+      </c>
+      <c r="S3" s="6">
+        <v>120</v>
+      </c>
+      <c r="T3" s="6">
+        <v>135</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H4" s="7">
+        <v>29.4</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>15</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>20</v>
+      </c>
+      <c r="O4" s="6">
+        <v>30</v>
+      </c>
+      <c r="P4" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>40</v>
+      </c>
+      <c r="R4" s="6">
+        <v>45</v>
+      </c>
+      <c r="S4" s="6">
+        <v>120</v>
+      </c>
+      <c r="T4" s="6">
+        <v>135</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z4" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H5" s="7">
+        <v>26.1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>15</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45</v>
+      </c>
+      <c r="M5" s="6">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6">
+        <v>20</v>
+      </c>
+      <c r="O5" s="6">
+        <v>30</v>
+      </c>
+      <c r="P5" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>40</v>
+      </c>
+      <c r="R5" s="6">
+        <v>45</v>
+      </c>
+      <c r="S5" s="6">
+        <v>120</v>
+      </c>
+      <c r="T5" s="6">
+        <v>135</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H6" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>15</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>45</v>
+      </c>
+      <c r="M6" s="6">
+        <v>10</v>
+      </c>
+      <c r="N6" s="6">
+        <v>20</v>
+      </c>
+      <c r="O6" s="6">
+        <v>30</v>
+      </c>
+      <c r="P6" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>40</v>
+      </c>
+      <c r="R6" s="6">
+        <v>45</v>
+      </c>
+      <c r="S6" s="6">
+        <v>120</v>
+      </c>
+      <c r="T6" s="6">
+        <v>135</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC6" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H7" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>15</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>45</v>
+      </c>
+      <c r="M7" s="6">
+        <v>10</v>
+      </c>
+      <c r="N7" s="6">
+        <v>20</v>
+      </c>
+      <c r="O7" s="6">
+        <v>30</v>
+      </c>
+      <c r="P7" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>40</v>
+      </c>
+      <c r="R7" s="6">
+        <v>45</v>
+      </c>
+      <c r="S7" s="6">
+        <v>120</v>
+      </c>
+      <c r="T7" s="6">
+        <v>135</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z7" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC7" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD7" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H8" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>15</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>45</v>
+      </c>
+      <c r="M8" s="6">
+        <v>10</v>
+      </c>
+      <c r="N8" s="6">
+        <v>20</v>
+      </c>
+      <c r="O8" s="6">
+        <v>30</v>
+      </c>
+      <c r="P8" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>40</v>
+      </c>
+      <c r="R8" s="6">
+        <v>45</v>
+      </c>
+      <c r="S8" s="6">
+        <v>120</v>
+      </c>
+      <c r="T8" s="6">
+        <v>135</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD8" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H9" s="7">
+        <v>22.5</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>15</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>45</v>
+      </c>
+      <c r="M9" s="6">
+        <v>10</v>
+      </c>
+      <c r="N9" s="6">
+        <v>20</v>
+      </c>
+      <c r="O9" s="6">
+        <v>30</v>
+      </c>
+      <c r="P9" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>40</v>
+      </c>
+      <c r="R9" s="6">
+        <v>45</v>
+      </c>
+      <c r="S9" s="6">
+        <v>120</v>
+      </c>
+      <c r="T9" s="6">
+        <v>135</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z9" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB9" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC9" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD9" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H10" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>15</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>45</v>
+      </c>
+      <c r="M10" s="6">
+        <v>10</v>
+      </c>
+      <c r="N10" s="6">
+        <v>20</v>
+      </c>
+      <c r="O10" s="6">
+        <v>30</v>
+      </c>
+      <c r="P10" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>40</v>
+      </c>
+      <c r="R10" s="6">
+        <v>45</v>
+      </c>
+      <c r="S10" s="6">
+        <v>120</v>
+      </c>
+      <c r="T10" s="6">
+        <v>135</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z10" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA10" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB10" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC10" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD10" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H11" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>15</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>45</v>
+      </c>
+      <c r="M11" s="6">
+        <v>10</v>
+      </c>
+      <c r="N11" s="6">
+        <v>20</v>
+      </c>
+      <c r="O11" s="6">
+        <v>30</v>
+      </c>
+      <c r="P11" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>40</v>
+      </c>
+      <c r="R11" s="6">
+        <v>45</v>
+      </c>
+      <c r="S11" s="6">
+        <v>120</v>
+      </c>
+      <c r="T11" s="6">
+        <v>135</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z11" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB11" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC11" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD11" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H12" s="7">
+        <v>29.4</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>15</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>45</v>
+      </c>
+      <c r="M12" s="6">
+        <v>10</v>
+      </c>
+      <c r="N12" s="6">
+        <v>20</v>
+      </c>
+      <c r="O12" s="6">
+        <v>30</v>
+      </c>
+      <c r="P12" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>40</v>
+      </c>
+      <c r="R12" s="6">
+        <v>45</v>
+      </c>
+      <c r="S12" s="6">
+        <v>120</v>
+      </c>
+      <c r="T12" s="6">
+        <v>135</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z12" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD12" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H13" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>15</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <v>45</v>
+      </c>
+      <c r="M13" s="6">
+        <v>10</v>
+      </c>
+      <c r="N13" s="6">
+        <v>20</v>
+      </c>
+      <c r="O13" s="6">
+        <v>30</v>
+      </c>
+      <c r="P13" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>40</v>
+      </c>
+      <c r="R13" s="6">
+        <v>45</v>
+      </c>
+      <c r="S13" s="6">
+        <v>120</v>
+      </c>
+      <c r="T13" s="6">
+        <v>135</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z13" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD13" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H14" s="7">
+        <v>27.6</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>15</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>45</v>
+      </c>
+      <c r="M14" s="6">
+        <v>10</v>
+      </c>
+      <c r="N14" s="6">
+        <v>20</v>
+      </c>
+      <c r="O14" s="6">
+        <v>30</v>
+      </c>
+      <c r="P14" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>40</v>
+      </c>
+      <c r="R14" s="6">
+        <v>45</v>
+      </c>
+      <c r="S14" s="6">
+        <v>120</v>
+      </c>
+      <c r="T14" s="6">
+        <v>135</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z14" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA14" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD14" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H15" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="6">
+        <v>15</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
+        <v>45</v>
+      </c>
+      <c r="M15" s="6">
+        <v>10</v>
+      </c>
+      <c r="N15" s="6">
+        <v>20</v>
+      </c>
+      <c r="O15" s="6">
+        <v>30</v>
+      </c>
+      <c r="P15" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>40</v>
+      </c>
+      <c r="R15" s="6">
+        <v>45</v>
+      </c>
+      <c r="S15" s="6">
+        <v>120</v>
+      </c>
+      <c r="T15" s="6">
+        <v>135</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y15" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z15" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA15" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC15" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H16" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>15</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>45</v>
+      </c>
+      <c r="M16" s="6">
+        <v>10</v>
+      </c>
+      <c r="N16" s="6">
+        <v>20</v>
+      </c>
+      <c r="O16" s="6">
+        <v>30</v>
+      </c>
+      <c r="P16" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>40</v>
+      </c>
+      <c r="R16" s="6">
+        <v>45</v>
+      </c>
+      <c r="S16" s="6">
+        <v>120</v>
+      </c>
+      <c r="T16" s="6">
+        <v>135</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y16" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z16" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA16" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -12309,13 +13779,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60942C2-4335-4670-987D-064E89656B98}">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -12413,6 +13883,398 @@
       </c>
       <c r="AF1" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H2" s="7">
+        <v>29.4</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>15</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>45</v>
+      </c>
+      <c r="M2" s="6">
+        <v>10</v>
+      </c>
+      <c r="N2" s="6">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6">
+        <v>30</v>
+      </c>
+      <c r="P2" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>40</v>
+      </c>
+      <c r="R2" s="6">
+        <v>45</v>
+      </c>
+      <c r="S2" s="6">
+        <v>120</v>
+      </c>
+      <c r="T2" s="6">
+        <v>135</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA2" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC2" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H3" s="7">
+        <v>30.5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>15</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>45</v>
+      </c>
+      <c r="M3" s="6">
+        <v>10</v>
+      </c>
+      <c r="N3" s="6">
+        <v>20</v>
+      </c>
+      <c r="O3" s="6">
+        <v>30</v>
+      </c>
+      <c r="P3" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>40</v>
+      </c>
+      <c r="R3" s="6">
+        <v>45</v>
+      </c>
+      <c r="S3" s="6">
+        <v>120</v>
+      </c>
+      <c r="T3" s="6">
+        <v>135</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H4" s="7">
+        <v>10.4</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>15</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>20</v>
+      </c>
+      <c r="O4" s="6">
+        <v>30</v>
+      </c>
+      <c r="P4" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>40</v>
+      </c>
+      <c r="R4" s="6">
+        <v>45</v>
+      </c>
+      <c r="S4" s="6">
+        <v>120</v>
+      </c>
+      <c r="T4" s="6">
+        <v>135</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z4" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H5" s="7">
+        <v>23.4</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>15</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45</v>
+      </c>
+      <c r="M5" s="6">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6">
+        <v>20</v>
+      </c>
+      <c r="O5" s="6">
+        <v>30</v>
+      </c>
+      <c r="P5" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>40</v>
+      </c>
+      <c r="R5" s="6">
+        <v>45</v>
+      </c>
+      <c r="S5" s="6">
+        <v>120</v>
+      </c>
+      <c r="T5" s="6">
+        <v>135</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -18881,7 +20743,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19967,13 +21829,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0D3A86-E412-427A-BCF1-BD33384ECBF3}">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -20071,6 +21933,1476 @@
       </c>
       <c r="AF1" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H2" s="7">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>15</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>45</v>
+      </c>
+      <c r="M2" s="6">
+        <v>10</v>
+      </c>
+      <c r="N2" s="6">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6">
+        <v>30</v>
+      </c>
+      <c r="P2" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>40</v>
+      </c>
+      <c r="R2" s="6">
+        <v>45</v>
+      </c>
+      <c r="S2" s="6">
+        <v>120</v>
+      </c>
+      <c r="T2" s="6">
+        <v>135</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA2" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC2" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H3" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>15</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>45</v>
+      </c>
+      <c r="M3" s="6">
+        <v>10</v>
+      </c>
+      <c r="N3" s="6">
+        <v>20</v>
+      </c>
+      <c r="O3" s="6">
+        <v>30</v>
+      </c>
+      <c r="P3" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>40</v>
+      </c>
+      <c r="R3" s="6">
+        <v>45</v>
+      </c>
+      <c r="S3" s="6">
+        <v>120</v>
+      </c>
+      <c r="T3" s="6">
+        <v>135</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H4" s="7">
+        <v>29.9</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>15</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>20</v>
+      </c>
+      <c r="O4" s="6">
+        <v>30</v>
+      </c>
+      <c r="P4" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>40</v>
+      </c>
+      <c r="R4" s="6">
+        <v>45</v>
+      </c>
+      <c r="S4" s="6">
+        <v>120</v>
+      </c>
+      <c r="T4" s="6">
+        <v>135</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z4" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H5" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>15</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45</v>
+      </c>
+      <c r="M5" s="6">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6">
+        <v>20</v>
+      </c>
+      <c r="O5" s="6">
+        <v>30</v>
+      </c>
+      <c r="P5" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>40</v>
+      </c>
+      <c r="R5" s="6">
+        <v>45</v>
+      </c>
+      <c r="S5" s="6">
+        <v>120</v>
+      </c>
+      <c r="T5" s="6">
+        <v>135</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H6" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>15</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>45</v>
+      </c>
+      <c r="M6" s="6">
+        <v>10</v>
+      </c>
+      <c r="N6" s="6">
+        <v>20</v>
+      </c>
+      <c r="O6" s="6">
+        <v>30</v>
+      </c>
+      <c r="P6" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>40</v>
+      </c>
+      <c r="R6" s="6">
+        <v>45</v>
+      </c>
+      <c r="S6" s="6">
+        <v>120</v>
+      </c>
+      <c r="T6" s="6">
+        <v>135</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC6" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H7" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>15</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>45</v>
+      </c>
+      <c r="M7" s="6">
+        <v>10</v>
+      </c>
+      <c r="N7" s="6">
+        <v>20</v>
+      </c>
+      <c r="O7" s="6">
+        <v>30</v>
+      </c>
+      <c r="P7" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>40</v>
+      </c>
+      <c r="R7" s="6">
+        <v>45</v>
+      </c>
+      <c r="S7" s="6">
+        <v>120</v>
+      </c>
+      <c r="T7" s="6">
+        <v>135</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z7" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC7" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD7" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H8" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>15</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>45</v>
+      </c>
+      <c r="M8" s="6">
+        <v>10</v>
+      </c>
+      <c r="N8" s="6">
+        <v>20</v>
+      </c>
+      <c r="O8" s="6">
+        <v>30</v>
+      </c>
+      <c r="P8" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>40</v>
+      </c>
+      <c r="R8" s="6">
+        <v>45</v>
+      </c>
+      <c r="S8" s="6">
+        <v>120</v>
+      </c>
+      <c r="T8" s="6">
+        <v>135</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD8" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H9" s="7">
+        <v>28.9</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>15</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>45</v>
+      </c>
+      <c r="M9" s="6">
+        <v>10</v>
+      </c>
+      <c r="N9" s="6">
+        <v>20</v>
+      </c>
+      <c r="O9" s="6">
+        <v>30</v>
+      </c>
+      <c r="P9" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>40</v>
+      </c>
+      <c r="R9" s="6">
+        <v>45</v>
+      </c>
+      <c r="S9" s="6">
+        <v>120</v>
+      </c>
+      <c r="T9" s="6">
+        <v>135</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z9" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB9" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC9" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD9" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H10" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>15</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>45</v>
+      </c>
+      <c r="M10" s="6">
+        <v>10</v>
+      </c>
+      <c r="N10" s="6">
+        <v>20</v>
+      </c>
+      <c r="O10" s="6">
+        <v>30</v>
+      </c>
+      <c r="P10" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>40</v>
+      </c>
+      <c r="R10" s="6">
+        <v>45</v>
+      </c>
+      <c r="S10" s="6">
+        <v>120</v>
+      </c>
+      <c r="T10" s="6">
+        <v>135</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z10" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA10" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB10" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC10" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD10" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H11" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>15</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>45</v>
+      </c>
+      <c r="M11" s="6">
+        <v>10</v>
+      </c>
+      <c r="N11" s="6">
+        <v>20</v>
+      </c>
+      <c r="O11" s="6">
+        <v>30</v>
+      </c>
+      <c r="P11" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>40</v>
+      </c>
+      <c r="R11" s="6">
+        <v>45</v>
+      </c>
+      <c r="S11" s="6">
+        <v>120</v>
+      </c>
+      <c r="T11" s="6">
+        <v>135</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z11" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB11" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC11" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD11" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H12" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>15</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>45</v>
+      </c>
+      <c r="M12" s="6">
+        <v>10</v>
+      </c>
+      <c r="N12" s="6">
+        <v>20</v>
+      </c>
+      <c r="O12" s="6">
+        <v>30</v>
+      </c>
+      <c r="P12" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>40</v>
+      </c>
+      <c r="R12" s="6">
+        <v>45</v>
+      </c>
+      <c r="S12" s="6">
+        <v>120</v>
+      </c>
+      <c r="T12" s="6">
+        <v>135</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z12" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD12" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H13" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>15</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <v>45</v>
+      </c>
+      <c r="M13" s="6">
+        <v>10</v>
+      </c>
+      <c r="N13" s="6">
+        <v>20</v>
+      </c>
+      <c r="O13" s="6">
+        <v>30</v>
+      </c>
+      <c r="P13" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>40</v>
+      </c>
+      <c r="R13" s="6">
+        <v>45</v>
+      </c>
+      <c r="S13" s="6">
+        <v>120</v>
+      </c>
+      <c r="T13" s="6">
+        <v>135</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z13" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD13" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H14" s="7">
+        <v>28.6</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>15</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>45</v>
+      </c>
+      <c r="M14" s="6">
+        <v>10</v>
+      </c>
+      <c r="N14" s="6">
+        <v>20</v>
+      </c>
+      <c r="O14" s="6">
+        <v>30</v>
+      </c>
+      <c r="P14" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>40</v>
+      </c>
+      <c r="R14" s="6">
+        <v>45</v>
+      </c>
+      <c r="S14" s="6">
+        <v>120</v>
+      </c>
+      <c r="T14" s="6">
+        <v>135</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z14" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA14" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD14" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H15" s="7">
+        <v>27.9</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="6">
+        <v>15</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
+        <v>45</v>
+      </c>
+      <c r="M15" s="6">
+        <v>10</v>
+      </c>
+      <c r="N15" s="6">
+        <v>20</v>
+      </c>
+      <c r="O15" s="6">
+        <v>30</v>
+      </c>
+      <c r="P15" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>40</v>
+      </c>
+      <c r="R15" s="6">
+        <v>45</v>
+      </c>
+      <c r="S15" s="6">
+        <v>120</v>
+      </c>
+      <c r="T15" s="6">
+        <v>135</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y15" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z15" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA15" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC15" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H16" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>15</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>45</v>
+      </c>
+      <c r="M16" s="6">
+        <v>10</v>
+      </c>
+      <c r="N16" s="6">
+        <v>20</v>
+      </c>
+      <c r="O16" s="6">
+        <v>30</v>
+      </c>
+      <c r="P16" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>40</v>
+      </c>
+      <c r="R16" s="6">
+        <v>45</v>
+      </c>
+      <c r="S16" s="6">
+        <v>120</v>
+      </c>
+      <c r="T16" s="6">
+        <v>135</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y16" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Z16" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AA16" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>